<commit_message>
WORKING.   produces well nested squares
</commit_message>
<xml_diff>
--- a/FY24 Projects DRAFT-v4.xlsx
+++ b/FY24 Projects DRAFT-v4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsteel01\Box\01 - P Drive 2\Employment\Goals\FY24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A244C53-6A11-4900-B6AE-94EFF93709FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA7971E-5092-422B-996C-DDBF7AD5606A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{A9DDD929-39F7-4D1E-ADFC-1FBC098A0B9E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t>task</t>
   </si>
@@ -50,24 +50,9 @@
     <t>Docline</t>
   </si>
   <si>
-    <t>SpineOMatic updated Alma cloud app (includes learning)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Read by QxMD - integration with Alma publishing profile </t>
-  </si>
-  <si>
     <t>course archiving</t>
   </si>
   <si>
-    <t>Medical and Vet Clinical OASIS feed into Alma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">loan rule Code4Lib article and collaboration with Getty </t>
-  </si>
-  <si>
-    <t>Leganto working group enhancements</t>
-  </si>
-  <si>
     <t>2024-02-15</t>
   </si>
   <si>
@@ -110,24 +95,9 @@
     <t>RHEL 7 to RHEL 9 for other servers</t>
   </si>
   <si>
-    <t>LOCKSS update (mostly leveraging LOCKSS support) and RHEL 9 upgrade</t>
-  </si>
-  <si>
-    <t>reading list student affordability - Phase I - process design and reading list creatoin</t>
-  </si>
-  <si>
-    <t>reading list student affordability - Phase II - testing and citation creation cloud app</t>
-  </si>
-  <si>
     <t>Ruby on Rails Udemy</t>
   </si>
   <si>
-    <t>ASpace name change</t>
-  </si>
-  <si>
-    <t>ELUNA presentation with Martha about reserves workflow enhancement</t>
-  </si>
-  <si>
     <t>2024-12-01</t>
   </si>
   <si>
@@ -146,10 +116,37 @@
     <t>2024-03-15</t>
   </si>
   <si>
-    <t>2024-05-41</t>
-  </si>
-  <si>
     <t>2024-06-01</t>
+  </si>
+  <si>
+    <t>2024-05-31</t>
+  </si>
+  <si>
+    <t>student reserves - Phase I</t>
+  </si>
+  <si>
+    <t>student reserves - Phase II</t>
+  </si>
+  <si>
+    <t>ELUNA presentation</t>
+  </si>
+  <si>
+    <t>LOCKSS upgrade and migration</t>
+  </si>
+  <si>
+    <t>OASIS</t>
+  </si>
+  <si>
+    <t>Leganto working group NERS</t>
+  </si>
+  <si>
+    <t>loan rule Code4Lib article</t>
+  </si>
+  <si>
+    <t>Read by QxMD</t>
+  </si>
+  <si>
+    <t>SpineOMatic Alma cloud app</t>
   </si>
 </sst>
 </file>
@@ -520,7 +517,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -541,7 +538,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -549,10 +546,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="D2">
         <v>3</v>
@@ -560,13 +557,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -574,13 +571,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -588,13 +585,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -602,13 +599,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D6">
         <v>3</v>
@@ -616,13 +613,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -630,13 +627,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -644,13 +641,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -658,13 +655,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -672,13 +669,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -686,13 +683,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="C12" s="3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D12">
         <v>3</v>
@@ -700,13 +697,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D13">
         <v>2</v>
@@ -714,13 +711,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -728,13 +725,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -742,13 +739,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D16">
         <v>2</v>

</xml_diff>